<commit_message>
Speaker added. Tweaks in screen
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3370" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3502" uniqueCount="113">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t xml:space="preserve">Temperature_Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buzz</t>
   </si>
 </sst>
 </file>
@@ -2130,7 +2136,23 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22"/>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="23"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Font sizes tweaks. Clean is now faster
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4528" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4906" uniqueCount="123">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1653,7 +1653,7 @@
         <v>87</v>
       </c>
       <c r="D5">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1691,7 +1691,7 @@
         <v>87</v>
       </c>
       <c r="D6">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E6">
         <v>1</v>

</xml_diff>

<commit_message>
Vdd readout routine added
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4906" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5172" uniqueCount="126">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -384,6 +384,15 @@
   </si>
   <si>
     <t xml:space="preserve">hPa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;V</t>
   </si>
 </sst>
 </file>
@@ -1625,9 +1634,13 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>64</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1862,7 +1875,7 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
@@ -1874,12 +1887,12 @@
         <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1891,12 +1904,12 @@
         <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -1908,32 +1921,32 @@
         <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -1942,117 +1955,117 @@
         <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
         <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
         <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
         <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>58</v>
@@ -2061,112 +2074,128 @@
         <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
         <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
         <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
         <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
         <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
         <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="23"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
4.2 eInk switched to gray2 mode
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5172" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5848" uniqueCount="129">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -393,6 +393,15 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;value&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
   </si>
 </sst>
 </file>
@@ -1626,10 +1635,10 @@
         <v>86</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -1666,10 +1675,10 @@
         <v>87</v>
       </c>
       <c r="D5">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -1704,10 +1713,10 @@
         <v>87</v>
       </c>
       <c r="D6">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -1898,13 +1907,13 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
         <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6">
@@ -2142,7 +2151,7 @@
         <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20">
@@ -2196,7 +2205,23 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23"/>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Displaying sd available space
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5848" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6476" uniqueCount="134">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -402,6 +402,21 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.kMGB</t>
   </si>
 </sst>
 </file>
@@ -1744,6 +1759,25 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7"/>
       <c r="I7" t="s">
         <v>64</v>
       </c>
@@ -1887,7 +1921,7 @@
         <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
         <v>45</v>
@@ -1904,7 +1938,7 @@
         <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
         <v>119</v>
@@ -1921,10 +1955,10 @@
         <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="E6" t="s">
         <v>46</v>
@@ -2176,7 +2210,7 @@
         <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
         <v>58</v>
@@ -2193,7 +2227,7 @@
         <v>124</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
         <v>58</v>
@@ -2210,16 +2244,50 @@
         <v>128</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="E23" t="s">
         <v>46</v>
       </c>
       <c r="F23" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Displaying info about sd errors
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6476" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6959" uniqueCount="135">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t xml:space="preserve">.kMGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Err</t>
   </si>
 </sst>
 </file>
@@ -2290,6 +2293,7 @@
         <v>59</v>
       </c>
     </row>
+    <row r="26"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Displaying date and time
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9365" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10269" uniqueCount="169">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -513,6 +513,15 @@
   </si>
   <si>
     <t xml:space="preserve">xxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-01-17 14:57&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">: -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. :-</t>
   </si>
 </sst>
 </file>
@@ -1948,9 +1957,13 @@
       <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="G9"/>
+      <c r="G9" t="s">
+        <v>168</v>
+      </c>
       <c r="H9"/>
-      <c r="I9"/>
+      <c r="I9" t="s">
+        <v>64</v>
+      </c>
       <c r="J9"/>
       <c r="L9" s="11" t="s">
         <v>6</v>
@@ -2489,7 +2502,7 @@
         <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>150</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30">

</xml_diff>

<commit_message>
Logger is now disabled on start up
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13612" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13941" uniqueCount="198">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -606,6 +606,9 @@
   </si>
   <si>
     <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.kMGB:ErOf</t>
   </si>
 </sst>
 </file>
@@ -1964,7 +1967,7 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">

</xml_diff>

<commit_message>
3d prints. Main screen amended. Last bar issue fixed
</commit_message>
<xml_diff>
--- a/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32CubeIDE/EnvSensor/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13941" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18105" uniqueCount="202">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -609,6 +609,18 @@
   </si>
   <si>
     <t xml:space="preserve">.kMGB:ErOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
   </si>
 </sst>
 </file>
@@ -1882,7 +1894,7 @@
         <v>87</v>
       </c>
       <c r="D5">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1920,7 +1932,7 @@
         <v>87</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2206,7 +2218,7 @@
         <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
@@ -2240,7 +2252,7 @@
         <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
@@ -2257,7 +2269,7 @@
         <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
         <v>58</v>
@@ -2274,7 +2286,7 @@
         <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -2291,7 +2303,7 @@
         <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D12" t="s">
         <v>58</v>
@@ -2308,7 +2320,7 @@
         <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
         <v>45</v>
@@ -2325,7 +2337,7 @@
         <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D14" t="s">
         <v>58</v>
@@ -2359,7 +2371,7 @@
         <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -2376,7 +2388,7 @@
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
         <v>58</v>
@@ -2393,7 +2405,7 @@
         <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D18" t="s">
         <v>45</v>
@@ -2410,7 +2422,7 @@
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D19" t="s">
         <v>58</v>
@@ -2427,7 +2439,7 @@
         <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
         <v>45</v>
@@ -2981,6 +2993,57 @@
       </c>
       <c r="F52" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>201</v>
+      </c>
+      <c r="C55" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F55" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>